<commit_message>
Complétion de la planification (Excel), ajout du JDB, modification de la liste des tâches
</commit_message>
<xml_diff>
--- a/Documentation/planification Initiale.xlsx
+++ b/Documentation/planification Initiale.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Tâche</t>
   </si>
@@ -40,12 +40,42 @@
   <si>
     <t>Nb Périodes</t>
   </si>
+  <si>
+    <t>Recherche d'informations</t>
+  </si>
+  <si>
+    <t>Estimation de la dose de travail</t>
+  </si>
+  <si>
+    <t>Recherche d'outils</t>
+  </si>
+  <si>
+    <t>Mise en place de l'environnement de travail</t>
+  </si>
+  <si>
+    <t>Développement du réseau neural</t>
+  </si>
+  <si>
+    <t>Développement du programme général</t>
+  </si>
+  <si>
+    <t>Entraînement final du réseau</t>
+  </si>
+  <si>
+    <t>Tests Finaux, Rendu</t>
+  </si>
+  <si>
+    <t>Vacances</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="ddd\ dd/mm"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,16 +83,146 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -70,12 +230,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,17 +617,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -381,22 +643,803 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="13">
+        <v>43147</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
       <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="16">
+        <v>43161</v>
+      </c>
+      <c r="D3" s="7">
+        <v>43132</v>
+      </c>
+      <c r="E3" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E3">
-        <v>1.02</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
+      <c r="F3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15">
+        <v>43166</v>
+      </c>
+      <c r="D4" s="8">
+        <v>43133</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14">
+        <v>43168</v>
+      </c>
+      <c r="D5" s="8">
+        <v>43134</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="27">
+        <v>43172</v>
+      </c>
+      <c r="D6" s="9">
+        <v>43135</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="29">
+        <v>43182</v>
+      </c>
+      <c r="D7" s="7">
+        <v>43136</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="32">
+        <v>43189</v>
+      </c>
+      <c r="D8" s="8">
+        <v>43137</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="28">
+        <v>43207</v>
+      </c>
+      <c r="D9" s="8">
+        <v>43138</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="37">
+        <v>43210</v>
+      </c>
+      <c r="D10" s="8">
+        <v>43139</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="8">
+        <v>43140</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="8">
+        <v>43141</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="9">
+        <v>43142</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="7">
+        <v>43143</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="8">
+        <v>43144</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="8">
+        <v>43145</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="8">
+        <v>43146</v>
+      </c>
+      <c r="E17" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="19">
+        <v>43147</v>
+      </c>
+      <c r="E18" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="8">
+        <v>43148</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="9">
+        <v>43149</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="10">
+        <v>43150</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="11">
+        <v>43151</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="11">
+        <v>43152</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="11">
+        <v>43153</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="11">
+        <v>43154</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="11">
+        <v>43155</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="12">
+        <v>43156</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="7">
+        <v>43157</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="8">
+        <v>43158</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="8">
+        <v>43159</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="8">
+        <v>43160</v>
+      </c>
+      <c r="E31" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="17">
+        <v>43161</v>
+      </c>
+      <c r="E32" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="8">
+        <v>43162</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="9">
+        <v>43163</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="7">
+        <v>43164</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="8">
+        <v>43165</v>
+      </c>
+      <c r="E36" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="21">
+        <v>43166</v>
+      </c>
+      <c r="E37" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="8">
+        <v>43167</v>
+      </c>
+      <c r="E38" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="25">
+        <v>43168</v>
+      </c>
+      <c r="E39" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="8">
+        <v>43169</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="9">
+        <v>43170</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="7">
+        <v>43171</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="23">
+        <v>43172</v>
+      </c>
+      <c r="E43" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="8">
+        <v>43173</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="8">
+        <v>43174</v>
+      </c>
+      <c r="E45" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="8">
+        <v>43175</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="8">
+        <v>43176</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="9">
+        <v>43177</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="7">
+        <v>43178</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="8">
+        <v>43179</v>
+      </c>
+      <c r="E50" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="8">
+        <v>43180</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="8">
+        <v>43181</v>
+      </c>
+      <c r="E52" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="30">
+        <v>43182</v>
+      </c>
+      <c r="E53" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="8">
+        <v>43183</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="9">
+        <v>43184</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="7">
+        <v>43185</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="8">
+        <v>43186</v>
+      </c>
+      <c r="E57" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="8">
+        <v>43187</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="8">
+        <v>43188</v>
+      </c>
+      <c r="E59" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="33">
+        <v>43189</v>
+      </c>
+      <c r="E60" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="8">
+        <v>43190</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="9">
+        <v>43191</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="10">
+        <v>43192</v>
+      </c>
+      <c r="E63" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="11">
+        <v>43193</v>
+      </c>
+      <c r="E64" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D65" s="11">
+        <v>43194</v>
+      </c>
+      <c r="E65" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="11">
+        <v>43195</v>
+      </c>
+      <c r="E66" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D67" s="11">
+        <v>43196</v>
+      </c>
+      <c r="E67" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D68" s="11">
+        <v>43197</v>
+      </c>
+      <c r="E68" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D69" s="12">
+        <v>43198</v>
+      </c>
+      <c r="E69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D70" s="10">
+        <v>43199</v>
+      </c>
+      <c r="E70" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D71" s="11">
+        <v>43200</v>
+      </c>
+      <c r="E71" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D72" s="11">
+        <v>43201</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D73" s="11">
+        <v>43202</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D74" s="11">
+        <v>43203</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D75" s="11">
+        <v>43204</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D76" s="12">
+        <v>43205</v>
+      </c>
+      <c r="E76" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D77" s="7">
+        <v>43206</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D78" s="35">
+        <v>43207</v>
+      </c>
+      <c r="E78" s="36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D79" s="8">
+        <v>43208</v>
+      </c>
+      <c r="E79" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D80" s="8">
+        <v>43209</v>
+      </c>
+      <c r="E80" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D81" s="38">
+        <v>43210</v>
+      </c>
+      <c r="E81" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D82" s="8">
+        <v>43211</v>
+      </c>
+      <c r="E82" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D83" s="9">
+        <v>43212</v>
+      </c>
+      <c r="E83" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D84" s="7">
+        <v>43213</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D85" s="8">
+        <v>43214</v>
+      </c>
+      <c r="E85" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D86" s="8">
+        <v>43215</v>
+      </c>
+      <c r="E86" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D87" s="8">
+        <v>43216</v>
+      </c>
+      <c r="E87" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D88" s="8">
+        <v>43217</v>
+      </c>
+      <c r="E88" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D89" s="8">
+        <v>43218</v>
+      </c>
+      <c r="E89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D90" s="9">
+        <v>43219</v>
+      </c>
+      <c r="E90" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D91" s="7">
+        <v>43220</v>
+      </c>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D92" s="8"/>
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D93" s="8"/>
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D94" s="8"/>
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D95" s="8"/>
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D96" s="8"/>
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97" s="9"/>
+      <c r="E97" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>